<commit_message>
Add comment to README about newly discovered dangers of editing dates directly in CSV using Excel; may as well show the changes in the loadfiles as well
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -385,7 +385,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,6 +841,12 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>41676</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.79166666666666663</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>

</xml_diff>